<commit_message>
added some notes to global
</commit_message>
<xml_diff>
--- a/datasources.xlsx
+++ b/datasources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toadstool\Documents\R\beachwater_tmu_procogia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016B54C6-6CEE-4DD1-8EF3-ECCEE1138DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43241B7B-4C72-4712-8E1D-78C14D7AD420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6DB6AE0-A0D2-4280-A14F-1BCD709767CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="108">
   <si>
     <t>ID</t>
   </si>
@@ -345,6 +345,21 @@
   </si>
   <si>
     <t>Wind speed (assuming yesterdays) -- hourly mean</t>
+  </si>
+  <si>
+    <t>Calculate</t>
+  </si>
+  <si>
+    <t>Yesterdays mean temp - hourly</t>
+  </si>
+  <si>
+    <t>yesterday and today</t>
+  </si>
+  <si>
+    <t>mean across 24h</t>
+  </si>
+  <si>
+    <t>https://www.ndbc.noaa.gov/data/realtime2/46131.txt</t>
   </si>
 </sst>
 </file>
@@ -696,26 +711,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B779C026-A2EF-46BB-952F-6599EE8DF272}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="86" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="86" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -729,25 +745,28 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>39</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>56</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -760,35 +779,35 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
       <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
         <v>37</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>57</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>80</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>81</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>82</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -802,19 +821,22 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" t="s">
-        <v>38</v>
-      </c>
       <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -827,35 +849,35 @@
       <c r="D4" t="s">
         <v>102</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>32</v>
       </c>
-      <c r="G4" t="s">
-        <v>38</v>
-      </c>
       <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" t="s">
         <v>37</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>58</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>98</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>99</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>100</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -868,20 +890,20 @@
       <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
       <c r="F5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="G5" t="s">
-        <v>38</v>
-      </c>
       <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -892,34 +914,34 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>35</v>
       </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
       <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" t="s">
         <v>37</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>59</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>84</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>85</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -929,14 +951,14 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>36</v>
       </c>
-      <c r="G7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -949,26 +971,26 @@
       <c r="D8" t="s">
         <v>19</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>27</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>49</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>31</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>87</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>88</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -981,29 +1003,29 @@
       <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>25</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>49</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>33</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>90</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>91</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>92</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1016,26 +1038,26 @@
       <c r="D10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>27</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>49</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>33</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>94</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>95</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1048,26 +1070,26 @@
       <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>27</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>49</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>33</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>87</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>88</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1080,20 +1102,20 @@
       <c r="D12" t="s">
         <v>17</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>25</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>44</v>
       </c>
-      <c r="G12" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1106,17 +1128,17 @@
       <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>26</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>30</v>
       </c>
-      <c r="G13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1129,20 +1151,20 @@
       <c r="D14" t="s">
         <v>20</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>26</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>45</v>
       </c>
-      <c r="G14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I14" t="s">
+      <c r="H14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -1155,20 +1177,20 @@
       <c r="D15" t="s">
         <v>23</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>28</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>46</v>
       </c>
-      <c r="G15" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="H15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1181,20 +1203,20 @@
       <c r="D16" t="s">
         <v>24</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>25</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>47</v>
       </c>
-      <c r="G16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="H16" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1204,14 +1226,14 @@
       <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>48</v>
       </c>
-      <c r="G17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1224,17 +1246,17 @@
       <c r="D18" t="s">
         <v>19</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>27</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>49</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8</v>
       </c>
@@ -1247,17 +1269,17 @@
       <c r="D19" t="s">
         <v>21</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>25</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>49</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
@@ -1270,17 +1292,17 @@
       <c r="D20" t="s">
         <v>22</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>27</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>49</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10</v>
       </c>
@@ -1293,17 +1315,17 @@
       <c r="D21" t="s">
         <v>13</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>27</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>49</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1316,20 +1338,20 @@
       <c r="D22" t="s">
         <v>17</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>25</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>51</v>
       </c>
-      <c r="G22" t="s">
-        <v>38</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="H22" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1342,17 +1364,20 @@
       <c r="D23" t="s">
         <v>18</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>26</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>30</v>
       </c>
-      <c r="G23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1365,20 +1390,20 @@
       <c r="D24" t="s">
         <v>20</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>26</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>52</v>
       </c>
-      <c r="G24" t="s">
-        <v>38</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="H24" t="s">
+        <v>38</v>
+      </c>
+      <c r="J24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -1391,20 +1416,20 @@
       <c r="D25" t="s">
         <v>23</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>28</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>53</v>
       </c>
-      <c r="G25" t="s">
-        <v>38</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="H25" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>5</v>
       </c>
@@ -1417,20 +1442,20 @@
       <c r="D26" t="s">
         <v>24</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>25</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>54</v>
       </c>
-      <c r="G26" t="s">
-        <v>38</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="H26" t="s">
+        <v>38</v>
+      </c>
+      <c r="J26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>6</v>
       </c>
@@ -1440,14 +1465,14 @@
       <c r="C27" t="s">
         <v>16</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>55</v>
       </c>
-      <c r="G27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7</v>
       </c>
@@ -1460,17 +1485,17 @@
       <c r="D28" t="s">
         <v>19</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>27</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>49</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>8</v>
       </c>
@@ -1483,17 +1508,17 @@
       <c r="D29" t="s">
         <v>21</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>25</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>49</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>9</v>
       </c>
@@ -1506,17 +1531,17 @@
       <c r="D30" t="s">
         <v>22</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>27</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>49</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1529,17 +1554,17 @@
       <c r="D31" t="s">
         <v>13</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>27</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>49</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1552,20 +1577,20 @@
       <c r="D32" t="s">
         <v>17</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>25</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>69</v>
       </c>
-      <c r="G32" t="s">
-        <v>38</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="H32" t="s">
+        <v>38</v>
+      </c>
+      <c r="J32" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -1578,17 +1603,17 @@
       <c r="D33" t="s">
         <v>18</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>26</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>30</v>
       </c>
-      <c r="G33" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1601,20 +1626,20 @@
       <c r="D34" t="s">
         <v>20</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>26</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>70</v>
       </c>
-      <c r="G34" t="s">
-        <v>38</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="H34" t="s">
+        <v>38</v>
+      </c>
+      <c r="J34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1627,20 +1652,20 @@
       <c r="D35" t="s">
         <v>23</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>28</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>71</v>
       </c>
-      <c r="G35" t="s">
-        <v>38</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="H35" t="s">
+        <v>38</v>
+      </c>
+      <c r="J35" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -1653,20 +1678,20 @@
       <c r="D36" t="s">
         <v>24</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>25</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>72</v>
       </c>
-      <c r="G36" t="s">
-        <v>38</v>
-      </c>
-      <c r="I36" t="s">
+      <c r="H36" t="s">
+        <v>38</v>
+      </c>
+      <c r="J36" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6</v>
       </c>
@@ -1676,14 +1701,14 @@
       <c r="C37" t="s">
         <v>73</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>74</v>
       </c>
-      <c r="G37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7</v>
       </c>
@@ -1696,17 +1721,17 @@
       <c r="D38" t="s">
         <v>19</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>27</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>49</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>8</v>
       </c>
@@ -1719,17 +1744,17 @@
       <c r="D39" t="s">
         <v>21</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>25</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>49</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9</v>
       </c>
@@ -1742,17 +1767,17 @@
       <c r="D40" t="s">
         <v>22</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>27</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>49</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>10</v>
       </c>
@@ -1765,13 +1790,13 @@
       <c r="D41" t="s">
         <v>13</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>27</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>49</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dynamic ui and styling
</commit_message>
<xml_diff>
--- a/datasources.xlsx
+++ b/datasources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toadstool\Documents\R\beachwater_tmu_procogia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43241B7B-4C72-4712-8E1D-78C14D7AD420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F9D069-47D9-4AA8-94FE-D3DE695459B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6DB6AE0-A0D2-4280-A14F-1BCD709767CC}"/>
+    <workbookView xWindow="4230" yWindow="1995" windowWidth="21600" windowHeight="11385" xr2:uid="{A6DB6AE0-A0D2-4280-A14F-1BCD709767CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B779C026-A2EF-46BB-952F-6599EE8DF272}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add in helper functions for all reactive values
</commit_message>
<xml_diff>
--- a/datasources.xlsx
+++ b/datasources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toadstool\Documents\R\beachwater_tmu_procogia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F9D069-47D9-4AA8-94FE-D3DE695459B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58090F2-76E9-49C9-BC5E-32B81C23C80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4230" yWindow="1995" windowWidth="21600" windowHeight="11385" xr2:uid="{A6DB6AE0-A0D2-4280-A14F-1BCD709767CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="111">
   <si>
     <t>ID</t>
   </si>
@@ -360,6 +360,15 @@
   </si>
   <si>
     <t>https://www.ndbc.noaa.gov/data/realtime2/46131.txt</t>
+  </si>
+  <si>
+    <t>[0,2.5]</t>
+  </si>
+  <si>
+    <t>(2.5,7.6]</t>
+  </si>
+  <si>
+    <t>(7.6,240]</t>
   </si>
 </sst>
 </file>
@@ -714,7 +723,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="K5" sqref="K5:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,6 +911,15 @@
       <c r="I5" t="s">
         <v>42</v>
       </c>
+      <c r="K5" t="s">
+        <v>108</v>
+      </c>
+      <c r="L5" t="s">
+        <v>109</v>
+      </c>
+      <c r="M5" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">

</xml_diff>